<commit_message>
bootstrap: add sys.path injection to scripts; centralize DATA_CRM via settings.paths; safer Make targets
</commit_message>
<xml_diff>
--- a/data_crm/sku_map_crm_20250813_v1.xlsx
+++ b/data_crm/sku_map_crm_20250813_v1.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/Documents/useful tables/GPT/GPT Python CRM/Sample files for data sctructure xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/Docs/kaspi_etl_kaspiapi/data_crm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41099333-F45A-E441-8AD4-F45C8F4F4397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F4C16B-2FA8-4541-9881-A31387B570AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27020" xr2:uid="{7C9349CC-F560-544D-BC0A-1A20AD96F1C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sku_Map_CRM_01" sheetId="3" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -513,7 +510,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -703,37 +700,37 @@
     <xf numFmtId="3" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -742,7 +739,7 @@
     <xf numFmtId="14" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -751,248 +748,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="24"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1455,6 +1210,198 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1501,6 +1448,56 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1514,1461 +1511,32 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="order 23.5.25"/>
-      <sheetName val="order 31.5.25"/>
-      <sheetName val="order 31.5.25 Fanye inqury"/>
-      <sheetName val="fannye 31.5.25"/>
-      <sheetName val="order 31.5.25 (2)"/>
-      <sheetName val="Sahar 16.6.25"/>
-      <sheetName val="Sahar 16.6.25 message"/>
-      <sheetName val="Calc sales"/>
-      <sheetName val="Sahar 16.7.25"/>
-      <sheetName val="Sahar 16.7.25 CRM"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10">
-        <row r="8">
-          <cell r="E8">
-            <v>3905</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9" t="str">
-            <v>RUSH nike BLACK</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>439</v>
-          </cell>
-          <cell r="F11" t="str">
-            <v>RUSH nike BLACK</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>36</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>75</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15">
-            <v>129</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>99</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>88</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19" t="str">
-            <v>Taitci black SHORT</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="E21">
-            <v>96</v>
-          </cell>
-          <cell r="F21" t="str">
-            <v>Taitci black SHORT</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>2</v>
-          </cell>
-          <cell r="F22" t="str">
-            <v>CL_NEW-CLO_MEN_TAICI_BLACK_S</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>10</v>
-          </cell>
-          <cell r="F23" t="str">
-            <v>CL_NEW-CLO_MEN_TAICI_BLACK_M</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>16</v>
-          </cell>
-          <cell r="F24" t="str">
-            <v>CL_NEW-CLO_MEN_TAICI_BLACK_L</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>27</v>
-          </cell>
-          <cell r="F25" t="str">
-            <v>CL_NEW-CLO_MEN_TAICI_BLACK_XL</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>23</v>
-          </cell>
-          <cell r="F26" t="str">
-            <v>CL_NEW-CLO_MEN_TAICI_BLACK_2XL</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="E27">
-            <v>18</v>
-          </cell>
-          <cell r="F27" t="str">
-            <v>CL_NEW-CLO_MEN_TAICI_BLACK_3XL</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29" t="str">
-            <v>Taitci white SHORT</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>192</v>
-          </cell>
-          <cell r="F31" t="str">
-            <v>Taitci white SHORT</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="E34">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>54</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>36</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39" t="str">
-            <v>LOSINA WHITE</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="E40">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>410</v>
-          </cell>
-          <cell r="F41" t="str">
-            <v>LOSINA WHITE</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>10</v>
-          </cell>
-          <cell r="F42" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_WHITE_S</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>43</v>
-          </cell>
-          <cell r="F43" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_WHITE_M</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>68</v>
-          </cell>
-          <cell r="F44" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_WHITE_L</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>116</v>
-          </cell>
-          <cell r="F45" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_WHITE_XL</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="E46">
-            <v>96</v>
-          </cell>
-          <cell r="F46" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_WHITE_2XL</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>77</v>
-          </cell>
-          <cell r="F47" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_WHITE_3XL</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49" t="str">
-            <v>LOSINA BLACK</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>170</v>
-          </cell>
-          <cell r="F51" t="str">
-            <v>LOSINA BLACK</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="E52">
-            <v>4</v>
-          </cell>
-          <cell r="F52" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_BLACK_S</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="E53">
-            <v>18</v>
-          </cell>
-          <cell r="F53" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_BLACK_M</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>28</v>
-          </cell>
-          <cell r="F54" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_BLACK_L</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>48</v>
-          </cell>
-          <cell r="F55" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_BLACK_XL</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>40</v>
-          </cell>
-          <cell r="F56" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_BLACK_2XL</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>32</v>
-          </cell>
-          <cell r="F57" t="str">
-            <v>CL_NEW-CLO_MEN_LEG_BLACK_3XL</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="E59" t="str">
-            <v>RUSH BERSERK BLACK</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>44</v>
-          </cell>
-          <cell r="F61" t="str">
-            <v>RUSH BERSERK BLACK</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="E65">
-            <v>16</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69" t="str">
-            <v>RUSH PRO COMBAT BLACK</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="E71">
-            <v>75</v>
-          </cell>
-          <cell r="F71" t="str">
-            <v>RUSH PRO COMBAT BLACK</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>2</v>
-          </cell>
-          <cell r="F72" t="str">
-            <v>CL_NEW-CLO_MEN_RUSH-PRO_BLACK_s</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>6</v>
-          </cell>
-          <cell r="F73" t="str">
-            <v>CL_NEW-CLO_MEN_RUSH-PRO_BLACK_M</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>13</v>
-          </cell>
-          <cell r="F74" t="str">
-            <v>CL_NEW-CLO_MEN_RUSH-PRO_BLACK_L</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>22</v>
-          </cell>
-          <cell r="F75" t="str">
-            <v>CL_NEW-CLO_MEN_RUSH-PRO_BLACK_XL</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>17</v>
-          </cell>
-          <cell r="F76" t="str">
-            <v>CL_NEW-CLO_MEN_RUSH-PRO_BLACK_2XL</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="E77">
-            <v>15</v>
-          </cell>
-          <cell r="F77" t="str">
-            <v>CL_NEW-CLO_MEN_RUSH-PRO_BLACK_3XL</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79" t="str">
-            <v>RUSH SPIDER BLACK</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>23</v>
-          </cell>
-          <cell r="F81" t="str">
-            <v>RUSH SPIDER BLACK</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="E84">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89" t="str">
-            <v>T-SHIRT  Black</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="E90">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>89</v>
-          </cell>
-          <cell r="F91" t="str">
-            <v>T-SHIRT  Black</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="E96">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99" t="str">
-            <v>T-SHIRT  Grey</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>19</v>
-          </cell>
-          <cell r="F101" t="str">
-            <v>T-SHIRT  Grey</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="E102">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="E103">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="E104">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="E105">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="E106">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="E107">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="E109" t="str">
-            <v>T-SHIRT BERSERK BLACK</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="E110">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="E111">
-            <v>121</v>
-          </cell>
-          <cell r="F111" t="str">
-            <v>T-SHIRT BERSERK BLACK</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="E112">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="E113">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="E114">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="E115">
-            <v>31</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="E116">
-            <v>39</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="E117">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="E119" t="str">
-            <v>T-SHIRT BERSERK white</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="E120">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="E121">
-            <v>51</v>
-          </cell>
-          <cell r="F121" t="str">
-            <v>T-SHIRT BERSERK white</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="E122">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="E123">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="E124">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="E125">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="E126">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="E127">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="E129" t="str">
-            <v>T-SHIRT BERSERK grey</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="E130">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="E131">
-            <v>53</v>
-          </cell>
-          <cell r="F131" t="str">
-            <v>T-SHIRT BERSERK grey</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="E132">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="E133">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="E134">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="E135">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="E136">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="137">
-          <cell r="E137">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="E139" t="str">
-            <v>T-SHIRT BERSERK BLACK-grey</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="E140">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="E141">
-            <v>27</v>
-          </cell>
-          <cell r="F141" t="str">
-            <v>T-SHIRT BERSERK BLACK-grey</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="E142">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="E143">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="E144">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="E145">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="E146">
-            <v>9</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="E147">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="E149" t="str">
-            <v>Suit 3 BLACK kids</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="E150">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="E151">
-            <v>20</v>
-          </cell>
-          <cell r="F151" t="str">
-            <v>Suit 3 BLACK kids</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="E152">
-            <v>1</v>
-          </cell>
-          <cell r="F152" t="str">
-            <v>CL_NEW-CLO_KIDS_KID-31_BLACK_22</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="E153">
-            <v>4</v>
-          </cell>
-          <cell r="F153" t="str">
-            <v>CL_NEW-CLO_KIDS_KID-31_BLACK_24</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="E154">
-            <v>6</v>
-          </cell>
-          <cell r="F154" t="str">
-            <v>CL_NEW-CLO_KIDS_KID-31_BLACK_26</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="E155">
-            <v>4</v>
-          </cell>
-          <cell r="F155" t="str">
-            <v>CL_NEW-CLO_KIDS_KID-31_BLACK_28</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="E156">
-            <v>5</v>
-          </cell>
-          <cell r="F156" t="str">
-            <v>CL_NEW-CLO_KIDS_KID-31_BLACK_30</v>
-          </cell>
-        </row>
-        <row r="158">
-          <cell r="E158" t="str">
-            <v>Suit 5 gray triangle kids</v>
-          </cell>
-        </row>
-        <row r="159">
-          <cell r="E159">
-            <v>53</v>
-          </cell>
-        </row>
-        <row r="160">
-          <cell r="E160">
-            <v>99</v>
-          </cell>
-          <cell r="F160" t="str">
-            <v>Suit 5 gray triangle kids</v>
-          </cell>
-        </row>
-        <row r="161">
-          <cell r="E161">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="162">
-          <cell r="E162">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="163">
-          <cell r="E163">
-            <v>34</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="E164">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="165">
-          <cell r="E165">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="167">
-          <cell r="E167" t="str">
-            <v>Suit 5 gray triangle</v>
-          </cell>
-        </row>
-        <row r="168">
-          <cell r="E168">
-            <v>55</v>
-          </cell>
-        </row>
-        <row r="169">
-          <cell r="E169">
-            <v>120</v>
-          </cell>
-          <cell r="F169" t="str">
-            <v>Suit 5 gray triangle</v>
-          </cell>
-        </row>
-        <row r="170">
-          <cell r="E170">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="171">
-          <cell r="E171">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="172">
-          <cell r="E172">
-            <v>23</v>
-          </cell>
-        </row>
-        <row r="173">
-          <cell r="E173">
-            <v>28</v>
-          </cell>
-        </row>
-        <row r="174">
-          <cell r="E174">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="175">
-          <cell r="E175">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="176">
-          <cell r="E176">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="178">
-          <cell r="E178" t="str">
-            <v>Suit 5 white-black</v>
-          </cell>
-        </row>
-        <row r="179">
-          <cell r="E179">
-            <v>60</v>
-          </cell>
-        </row>
-        <row r="180">
-          <cell r="E180">
-            <v>250</v>
-          </cell>
-          <cell r="F180" t="str">
-            <v>Suit 5 white-black</v>
-          </cell>
-        </row>
-        <row r="181">
-          <cell r="E181">
-            <v>0</v>
-          </cell>
-          <cell r="F181" t="str">
-            <v>CL_OC_MEN_BELI51_WHITE_S</v>
-          </cell>
-        </row>
-        <row r="182">
-          <cell r="E182">
-            <v>0</v>
-          </cell>
-          <cell r="F182" t="str">
-            <v>CL_OC_MEN_BELI51_WHITE_M</v>
-          </cell>
-        </row>
-        <row r="183">
-          <cell r="E183">
-            <v>0</v>
-          </cell>
-          <cell r="F183" t="str">
-            <v>CL_OC_MEN_BELI51_WHITE_L</v>
-          </cell>
-        </row>
-        <row r="184">
-          <cell r="E184">
-            <v>100</v>
-          </cell>
-          <cell r="F184" t="str">
-            <v>CL_OC_MEN_BELI51_WHITE_XL</v>
-          </cell>
-        </row>
-        <row r="185">
-          <cell r="E185">
-            <v>50</v>
-          </cell>
-          <cell r="F185" t="str">
-            <v>CL_OC_MEN_BELI51_WHITE_2XL</v>
-          </cell>
-        </row>
-        <row r="186">
-          <cell r="E186">
-            <v>75</v>
-          </cell>
-          <cell r="F186" t="str">
-            <v>CL_OC_MEN_BELI51_WHITE_3XL</v>
-          </cell>
-        </row>
-        <row r="187">
-          <cell r="E187">
-            <v>25</v>
-          </cell>
-          <cell r="F187" t="str">
-            <v>CL_OC_MEN_BELI51_WHITE_4XL</v>
-          </cell>
-        </row>
-        <row r="189">
-          <cell r="E189" t="str">
-            <v>Suit 5 white-black</v>
-          </cell>
-        </row>
-        <row r="190">
-          <cell r="E190">
-            <v>60</v>
-          </cell>
-        </row>
-        <row r="191">
-          <cell r="E191">
-            <v>200</v>
-          </cell>
-        </row>
-        <row r="192">
-          <cell r="E192">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="193">
-          <cell r="E193">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="194">
-          <cell r="E194">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="195">
-          <cell r="E195">
-            <v>80</v>
-          </cell>
-        </row>
-        <row r="196">
-          <cell r="E196">
-            <v>40</v>
-          </cell>
-        </row>
-        <row r="197">
-          <cell r="E197">
-            <v>60</v>
-          </cell>
-        </row>
-        <row r="198">
-          <cell r="E198">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="201">
-          <cell r="E201" t="str">
-            <v>Suit 5 white-black</v>
-          </cell>
-        </row>
-        <row r="202">
-          <cell r="E202">
-            <v>60</v>
-          </cell>
-        </row>
-        <row r="203">
-          <cell r="E203">
-            <v>50</v>
-          </cell>
-        </row>
-        <row r="204">
-          <cell r="E204">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="205">
-          <cell r="E205">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="206">
-          <cell r="E206">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="207">
-          <cell r="E207">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="208">
-          <cell r="E208">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="209">
-          <cell r="E209">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="210">
-          <cell r="E210">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="212">
-          <cell r="E212" t="str">
-            <v>RUSH nike BLACK</v>
-          </cell>
-        </row>
-        <row r="213">
-          <cell r="E213">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="214">
-          <cell r="E214">
-            <v>57</v>
-          </cell>
-        </row>
-        <row r="215">
-          <cell r="E215">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="216">
-          <cell r="E216">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="217">
-          <cell r="E217">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="218">
-          <cell r="E218">
-            <v>57</v>
-          </cell>
-        </row>
-        <row r="219">
-          <cell r="E219">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="220">
-          <cell r="E220">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="222">
-          <cell r="E222" t="str">
-            <v>Suit 5 PRINT</v>
-          </cell>
-        </row>
-        <row r="223">
-          <cell r="E223">
-            <v>47</v>
-          </cell>
-        </row>
-        <row r="224">
-          <cell r="E224">
-            <v>450</v>
-          </cell>
-          <cell r="F224" t="str">
-            <v>Suit 5 PRINT</v>
-          </cell>
-        </row>
-        <row r="225">
-          <cell r="E225">
-            <v>10</v>
-          </cell>
-          <cell r="F225" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_S</v>
-          </cell>
-        </row>
-        <row r="226">
-          <cell r="E226">
-            <v>30</v>
-          </cell>
-          <cell r="F226" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_M</v>
-          </cell>
-        </row>
-        <row r="227">
-          <cell r="E227">
-            <v>60</v>
-          </cell>
-          <cell r="F227" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_L</v>
-          </cell>
-        </row>
-        <row r="228">
-          <cell r="E228">
-            <v>135</v>
-          </cell>
-          <cell r="F228" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_XL</v>
-          </cell>
-        </row>
-        <row r="229">
-          <cell r="E229">
-            <v>85</v>
-          </cell>
-          <cell r="F229" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_2XL</v>
-          </cell>
-        </row>
-        <row r="230">
-          <cell r="E230">
-            <v>75</v>
-          </cell>
-          <cell r="F230" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_3XL</v>
-          </cell>
-        </row>
-        <row r="231">
-          <cell r="E231">
-            <v>55</v>
-          </cell>
-          <cell r="F231" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_4XL</v>
-          </cell>
-        </row>
-        <row r="233">
-          <cell r="E233" t="str">
-            <v>Suit 5 PRINT</v>
-          </cell>
-        </row>
-        <row r="234">
-          <cell r="E234">
-            <v>47</v>
-          </cell>
-        </row>
-        <row r="235">
-          <cell r="E235">
-            <v>450</v>
-          </cell>
-          <cell r="F235" t="str">
-            <v>Suit 5 PRINT</v>
-          </cell>
-        </row>
-        <row r="236">
-          <cell r="E236">
-            <v>10</v>
-          </cell>
-          <cell r="F236" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_S</v>
-          </cell>
-        </row>
-        <row r="237">
-          <cell r="E237">
-            <v>30</v>
-          </cell>
-          <cell r="F237" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_M</v>
-          </cell>
-        </row>
-        <row r="238">
-          <cell r="E238">
-            <v>60</v>
-          </cell>
-          <cell r="F238" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_L</v>
-          </cell>
-        </row>
-        <row r="239">
-          <cell r="E239">
-            <v>135</v>
-          </cell>
-          <cell r="F239" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_XL</v>
-          </cell>
-        </row>
-        <row r="240">
-          <cell r="E240">
-            <v>85</v>
-          </cell>
-          <cell r="F240" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_2XL</v>
-          </cell>
-        </row>
-        <row r="241">
-          <cell r="E241">
-            <v>75</v>
-          </cell>
-          <cell r="F241" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_3XL</v>
-          </cell>
-        </row>
-        <row r="242">
-          <cell r="E242">
-            <v>55</v>
-          </cell>
-          <cell r="F242" t="str">
-            <v>CL_OC_MEN_PRINT51_BLACK_4XL</v>
-          </cell>
-        </row>
-        <row r="249">
-          <cell r="E249" t="str">
-            <v>RUSH nike BLACK</v>
-          </cell>
-        </row>
-        <row r="250">
-          <cell r="E250">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="251">
-          <cell r="E251">
-            <v>200</v>
-          </cell>
-        </row>
-        <row r="253">
-          <cell r="E253">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="254">
-          <cell r="E254">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="255">
-          <cell r="E255">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="256">
-          <cell r="E256">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="257">
-          <cell r="E257">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="260">
-          <cell r="E260" t="str">
-            <v>RUSH nike BLACK</v>
-          </cell>
-        </row>
-        <row r="261">
-          <cell r="E261">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="262">
-          <cell r="E262">
-            <v>200</v>
-          </cell>
-        </row>
-        <row r="264">
-          <cell r="E264">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="265">
-          <cell r="E265">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="266">
-          <cell r="E266">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="267">
-          <cell r="E267">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="268">
-          <cell r="E268">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="272">
-          <cell r="E272" t="str">
-            <v>RUSH nike BLACK</v>
-          </cell>
-        </row>
-        <row r="273">
-          <cell r="E273">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="274">
-          <cell r="E274">
-            <v>1300</v>
-          </cell>
-        </row>
-        <row r="276">
-          <cell r="E276">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="277">
-          <cell r="E277">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="278">
-          <cell r="E278">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="279">
-          <cell r="E279">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="280">
-          <cell r="E280">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1334618A-E330-174F-BB65-786393C364B2}" name="Sku_Map_CRM_1" displayName="Sku_Map_CRM_1" ref="A1:T72" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1334618A-E330-174F-BB65-786393C364B2}" name="Sku_Map_CRM_1" displayName="Sku_Map_CRM_1" ref="A1:T72" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A1:T72" xr:uid="{1334618A-E330-174F-BB65-786393C364B2}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{DC43D604-1D92-2A4C-8C16-3E5C8D3FE865}" name="SKU_ID" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{54E0BF40-120F-9044-91A9-488943DCB960}" name="SKU_key" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{DC43D604-1D92-2A4C-8C16-3E5C8D3FE865}" name="SKU_ID" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{54E0BF40-120F-9044-91A9-488943DCB960}" name="SKU_key" dataDxfId="18">
       <calculatedColumnFormula>UPPER(_xlfn.TEXTJOIN("_",TRUE,Sku_Map_CRM_1[[#This Row],[Product_Type]],Sku_Map_CRM_1[[#This Row],[Sub_Category]],Sku_Map_CRM_1[[#This Row],[Brend]],Sku_Map_CRM_1[[#This Row],[Gender]],Sku_Map_CRM_1[[#This Row],[Model]],Sku_Map_CRM_1[[#This Row],[Color]],))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{867A37EE-85E0-0843-9C41-EC366B8D7624}" name="MY_SIZE" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{38EF2E33-2413-2E46-9385-2A9912B7A393}" name="Stock_before" dataDxfId="3">
-      <calculatedColumnFormula>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{A4AA7900-5271-E24B-BC6D-D20BAEC227C0}" name="stock_10.8.25" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{2A4985EA-17B0-654B-AF09-F25664863103}" name="Sales_start_date" dataDxfId="0"/>
-    <tableColumn id="19" xr3:uid="{9FDB698A-7138-8245-9315-AA20BA18AF64}" name="Sold _since_start" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{219EFFC5-706B-3C48-99C8-E7566FB53B07}" name="Kaspi_name_core" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{745910D2-9F35-9942-B89A-E869D2348CF3}" name="RECOMMENDED_RETAIL_PRICE" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{6F26ECE7-4F1B-0049-AF5E-43F034CB65B5}" name="Product_Type" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{B988F81B-D429-B442-BF33-BF6E709CF83B}" name="Sub_Category" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{E996996C-3FDA-8848-B38C-CF159D21087E}" name="Brend" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{47CCCA8D-E62D-324B-BA37-801072C4A546}" name="Model" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{E2E0C7E8-B952-8B41-BDC4-D07B8CFCA333}" name="Color" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{998499EC-B995-9D49-9934-7E20B9A08D72}" name="Gender" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{C3B390E4-AC8D-0F45-862D-3338F014137C}" name="Season" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{BAD17C33-C13B-3A4A-A221-F4B1B7D6CAAD}" name="BaseCost_CNY" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{0C329DB3-A9F5-BF4F-904D-3B9F1AE90D11}" name="Weight_kg" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{235B47FB-8EF3-B448-ABBD-972075FFB032}" name="VENDOR_ID" dataDxfId="9"/>
-    <tableColumn id="18" xr3:uid="{53E4C350-126D-7E45-BED2-AB6F3A2E3F1E}" name="Store_name" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{867A37EE-85E0-0843-9C41-EC366B8D7624}" name="MY_SIZE" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{38EF2E33-2413-2E46-9385-2A9912B7A393}" name="Stock_before" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{A4AA7900-5271-E24B-BC6D-D20BAEC227C0}" name="stock_10.8.25" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{2A4985EA-17B0-654B-AF09-F25664863103}" name="Sales_start_date" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{9FDB698A-7138-8245-9315-AA20BA18AF64}" name="Sold _since_start" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{219EFFC5-706B-3C48-99C8-E7566FB53B07}" name="Kaspi_name_core" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{745910D2-9F35-9942-B89A-E869D2348CF3}" name="RECOMMENDED_RETAIL_PRICE" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{6F26ECE7-4F1B-0049-AF5E-43F034CB65B5}" name="Product_Type" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{B988F81B-D429-B442-BF33-BF6E709CF83B}" name="Sub_Category" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{E996996C-3FDA-8848-B38C-CF159D21087E}" name="Brend" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{47CCCA8D-E62D-324B-BA37-801072C4A546}" name="Model" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{E2E0C7E8-B952-8B41-BDC4-D07B8CFCA333}" name="Color" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{998499EC-B995-9D49-9934-7E20B9A08D72}" name="Gender" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{C3B390E4-AC8D-0F45-862D-3338F014137C}" name="Season" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{BAD17C33-C13B-3A4A-A221-F4B1B7D6CAAD}" name="BaseCost_CNY" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{0C329DB3-A9F5-BF4F-904D-3B9F1AE90D11}" name="Weight_kg" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{235B47FB-8EF3-B448-ABBD-972075FFB032}" name="VENDOR_ID" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{53E4C350-126D-7E45-BED2-AB6F3A2E3F1E}" name="Store_name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3274,7 +1842,7 @@
   <dimension ref="A1:T72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16:R28"/>
+      <selection activeCell="D2" sqref="D2:D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
@@ -3366,7 +1934,6 @@
         <v>14</v>
       </c>
       <c r="D2" s="11">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E2" s="11">
@@ -3424,7 +1991,6 @@
         <v>22</v>
       </c>
       <c r="D3" s="11">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E3" s="11">
@@ -3482,7 +2048,6 @@
         <v>23</v>
       </c>
       <c r="D4" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E4" s="18">
@@ -3540,7 +2105,6 @@
         <v>24</v>
       </c>
       <c r="D5" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E5" s="18">
@@ -3598,7 +2162,6 @@
         <v>25</v>
       </c>
       <c r="D6" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E6" s="18">
@@ -3656,7 +2219,6 @@
         <v>26</v>
       </c>
       <c r="D7" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E7" s="18">
@@ -3714,7 +2276,6 @@
         <v>27</v>
       </c>
       <c r="D8" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E8" s="18">
@@ -3772,7 +2333,6 @@
         <v>14</v>
       </c>
       <c r="D9" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E9" s="18">
@@ -3832,7 +2392,6 @@
         <v>22</v>
       </c>
       <c r="D10" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E10" s="18">
@@ -3892,7 +2451,6 @@
         <v>23</v>
       </c>
       <c r="D11" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E11" s="18">
@@ -3952,7 +2510,6 @@
         <v>24</v>
       </c>
       <c r="D12" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>100</v>
       </c>
       <c r="E12" s="18">
@@ -4012,7 +2569,6 @@
         <v>25</v>
       </c>
       <c r="D13" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>50</v>
       </c>
       <c r="E13" s="18">
@@ -4072,7 +2628,6 @@
         <v>26</v>
       </c>
       <c r="D14" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>75</v>
       </c>
       <c r="E14" s="18">
@@ -4132,7 +2687,6 @@
         <v>27</v>
       </c>
       <c r="D15" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>25</v>
       </c>
       <c r="E15" s="18">
@@ -4192,7 +2746,6 @@
         <v>0</v>
       </c>
       <c r="D16" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E16" s="18">
@@ -4250,7 +2803,6 @@
         <v>0</v>
       </c>
       <c r="D17" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E17" s="18">
@@ -4308,7 +2860,6 @@
         <v>0</v>
       </c>
       <c r="D18" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E18" s="18">
@@ -4366,7 +2917,6 @@
         <v>0</v>
       </c>
       <c r="D19" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E19" s="18">
@@ -4424,7 +2974,6 @@
         <v>0</v>
       </c>
       <c r="D20" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E20" s="18">
@@ -4482,7 +3031,6 @@
         <v>0</v>
       </c>
       <c r="D21" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E21" s="18">
@@ -4540,7 +3088,6 @@
         <v>0</v>
       </c>
       <c r="D22" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E22" s="18">
@@ -4599,7 +3146,6 @@
         <v>0</v>
       </c>
       <c r="D23" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E23" s="18">
@@ -4655,7 +3201,6 @@
         <v>0</v>
       </c>
       <c r="D24" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E24" s="18">
@@ -4711,7 +3256,6 @@
         <v>0</v>
       </c>
       <c r="D25" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E25" s="18">
@@ -4767,7 +3311,6 @@
         <v>0</v>
       </c>
       <c r="D26" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E26" s="18">
@@ -4823,7 +3366,6 @@
         <v>0</v>
       </c>
       <c r="D27" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E27" s="18">
@@ -4879,7 +3421,6 @@
         <v>0</v>
       </c>
       <c r="D28" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E28" s="18">
@@ -4935,7 +3476,6 @@
         <v>0</v>
       </c>
       <c r="D29" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E29" s="18">
@@ -4991,7 +3531,6 @@
         <v>0</v>
       </c>
       <c r="D30" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E30" s="18">
@@ -5047,7 +3586,6 @@
         <v>14</v>
       </c>
       <c r="D31" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E31" s="18">
@@ -5105,7 +3643,6 @@
         <v>22</v>
       </c>
       <c r="D32" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E32" s="18">
@@ -5163,7 +3700,6 @@
         <v>23</v>
       </c>
       <c r="D33" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E33" s="18">
@@ -5221,7 +3757,6 @@
         <v>24</v>
       </c>
       <c r="D34" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E34" s="18">
@@ -5279,7 +3814,6 @@
         <v>25</v>
       </c>
       <c r="D35" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E35" s="18">
@@ -5337,7 +3871,6 @@
         <v>26</v>
       </c>
       <c r="D36" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>0</v>
       </c>
       <c r="E36" s="18">
@@ -5395,7 +3928,6 @@
         <v>14</v>
       </c>
       <c r="D37" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>2</v>
       </c>
       <c r="E37" s="18">
@@ -5453,7 +3985,6 @@
         <v>22</v>
       </c>
       <c r="D38" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>6</v>
       </c>
       <c r="E38" s="18">
@@ -5511,7 +4042,6 @@
         <v>23</v>
       </c>
       <c r="D39" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>13</v>
       </c>
       <c r="E39" s="18">
@@ -5569,7 +4099,6 @@
         <v>24</v>
       </c>
       <c r="D40" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>22</v>
       </c>
       <c r="E40" s="18">
@@ -5627,7 +4156,6 @@
         <v>25</v>
       </c>
       <c r="D41" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>17</v>
       </c>
       <c r="E41" s="18">
@@ -5685,7 +4213,6 @@
         <v>26</v>
       </c>
       <c r="D42" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>15</v>
       </c>
       <c r="E42" s="18">
@@ -5743,7 +4270,6 @@
         <v>22</v>
       </c>
       <c r="D43" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>1</v>
       </c>
       <c r="E43" s="18">
@@ -5801,7 +4327,6 @@
         <v>24</v>
       </c>
       <c r="D44" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>4</v>
       </c>
       <c r="E44" s="18">
@@ -5859,7 +4384,6 @@
         <v>26</v>
       </c>
       <c r="D45" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>6</v>
       </c>
       <c r="E45" s="18">
@@ -5917,7 +4441,6 @@
         <v>28</v>
       </c>
       <c r="D46" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>4</v>
       </c>
       <c r="E46" s="18">
@@ -5975,7 +4498,6 @@
         <v>30</v>
       </c>
       <c r="D47" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>5</v>
       </c>
       <c r="E47" s="18">
@@ -6033,7 +4555,6 @@
         <v>14</v>
       </c>
       <c r="D48" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>4</v>
       </c>
       <c r="E48" s="18">
@@ -6091,7 +4612,6 @@
         <v>22</v>
       </c>
       <c r="D49" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>18</v>
       </c>
       <c r="E49" s="18">
@@ -6149,7 +4669,6 @@
         <v>23</v>
       </c>
       <c r="D50" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>28</v>
       </c>
       <c r="E50" s="18">
@@ -6207,7 +4726,6 @@
         <v>24</v>
       </c>
       <c r="D51" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>48</v>
       </c>
       <c r="E51" s="18">
@@ -6265,7 +4783,6 @@
         <v>25</v>
       </c>
       <c r="D52" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>40</v>
       </c>
       <c r="E52" s="18">
@@ -6323,7 +4840,6 @@
         <v>26</v>
       </c>
       <c r="D53" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>32</v>
       </c>
       <c r="E53" s="18">
@@ -6381,7 +4897,6 @@
         <v>14</v>
       </c>
       <c r="D54" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>2</v>
       </c>
       <c r="E54" s="18">
@@ -6439,7 +4954,6 @@
         <v>22</v>
       </c>
       <c r="D55" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>10</v>
       </c>
       <c r="E55" s="18">
@@ -6497,7 +5011,6 @@
         <v>23</v>
       </c>
       <c r="D56" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>16</v>
       </c>
       <c r="E56" s="18">
@@ -6555,7 +5068,6 @@
         <v>24</v>
       </c>
       <c r="D57" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>27</v>
       </c>
       <c r="E57" s="18">
@@ -6613,7 +5125,6 @@
         <v>25</v>
       </c>
       <c r="D58" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>23</v>
       </c>
       <c r="E58" s="18">
@@ -6671,7 +5182,6 @@
         <v>26</v>
       </c>
       <c r="D59" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>18</v>
       </c>
       <c r="E59" s="18">
@@ -6729,7 +5239,6 @@
         <v>14</v>
       </c>
       <c r="D60" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>10</v>
       </c>
       <c r="E60" s="18">
@@ -6787,7 +5296,6 @@
         <v>22</v>
       </c>
       <c r="D61" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>43</v>
       </c>
       <c r="E61" s="18">
@@ -6845,7 +5353,6 @@
         <v>23</v>
       </c>
       <c r="D62" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>68</v>
       </c>
       <c r="E62" s="18">
@@ -6903,7 +5410,6 @@
         <v>24</v>
       </c>
       <c r="D63" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>116</v>
       </c>
       <c r="E63" s="18">
@@ -6961,7 +5467,6 @@
         <v>25</v>
       </c>
       <c r="D64" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>96</v>
       </c>
       <c r="E64" s="18">
@@ -7019,7 +5524,6 @@
         <v>26</v>
       </c>
       <c r="D65" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>77</v>
       </c>
       <c r="E65" s="18">
@@ -7077,7 +5581,6 @@
         <v>14</v>
       </c>
       <c r="D66" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>20</v>
       </c>
       <c r="E66" s="18">
@@ -7137,7 +5640,6 @@
         <v>22</v>
       </c>
       <c r="D67" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>60</v>
       </c>
       <c r="E67" s="18">
@@ -7197,7 +5699,6 @@
         <v>23</v>
       </c>
       <c r="D68" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>120</v>
       </c>
       <c r="E68" s="18">
@@ -7257,7 +5758,6 @@
         <v>24</v>
       </c>
       <c r="D69" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>270</v>
       </c>
       <c r="E69" s="18">
@@ -7317,7 +5817,6 @@
         <v>25</v>
       </c>
       <c r="D70" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>170</v>
       </c>
       <c r="E70" s="18">
@@ -7377,7 +5876,6 @@
         <v>26</v>
       </c>
       <c r="D71" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>150</v>
       </c>
       <c r="E71" s="18">
@@ -7437,7 +5935,6 @@
         <v>27</v>
       </c>
       <c r="D72" s="18">
-        <f>SUMIF('[1]Sahar 16.7.25 CRM'!$F:$F,Sku_Map_CRM_1[[#This Row],[SKU_ID]],'[1]Sahar 16.7.25 CRM'!$E:$E)</f>
         <v>110</v>
       </c>
       <c r="E72" s="18">

</xml_diff>